<commit_message>
Casos de prueba actualizado
</commit_message>
<xml_diff>
--- a/docs/NoteBook/Test plans and data/CASOS DE PRUEBA CICLO2.xlsx
+++ b/docs/NoteBook/Test plans and data/CASOS DE PRUEBA CICLO2.xlsx
@@ -107,6 +107,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Salida:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> identificar y mostrar que fue adicionada una nueva linea de codigo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Entrada:</t>
     </r>
     <r>
@@ -117,7 +140,53 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> adicionar una linea en el segundo programa </t>
+      <t xml:space="preserve"> eliminar una o varias lineas de código en el programa de versión nueva.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entrada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> adicionar una o varias lineas en el segundo programa o versión nueva.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entrada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Subir o leer los 2 programas (versión antigua y versión nueva)</t>
     </r>
   </si>
   <si>
@@ -140,7 +209,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> identificar y mostrar que fue adicionada una nueva linea de codigo</t>
+      <t xml:space="preserve"> Mostrar el total de LOC del programa No. 2 o versión nueva.</t>
     </r>
   </si>
   <si>
@@ -163,7 +232,201 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> eliminar una o varias lineas de código en el programa de versión nueva.</t>
+      <t xml:space="preserve"> modificar y eliminar lineas de la vesión nueva.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salida:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mostrar en pantalla el efecto realizado, ya sea linea modifica, eliminada o nueva.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salida:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Resultado de lineas comparadas, esta salida depende de los criterios de conteo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salida:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mostrar mensaje de excepción, explicando los sucedido.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entrada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Subir un programa de diferentes nombres o extensiones</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salida:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mostrar mensaje de error o excepciones</t>
+    </r>
+  </si>
+  <si>
+    <t>CASOS DE PRUEBA CAJA BLANCA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entradas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Entrar 2 programas diferentes con ext .java</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entradas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Modificar, adicionar y eliminar una linea de código en la version nueva del programa comprado.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entrada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Subir 1 solo programa de los 2 a comparar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entrada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> adicionar una linea en el programa versión nueva</t>
     </r>
   </si>
   <si>
@@ -186,30 +449,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>identificar y mostrar la(s) lineas eliminadas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entrada:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> adicionar una o varias lineas en el segundo programa o versión nueva.</t>
+      <t>identificar la(s) lineas eliminadas</t>
     </r>
   </si>
   <si>
@@ -232,53 +472,72 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> enumerar y mostrar lineas adicionadas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Salida: enumerar e </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>identificar y mostrar la(s) lineas eliminadas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entrada:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Subir o leer los 2 programas (versión antigua y versión nueva)</t>
+      <t xml:space="preserve"> mostrar el número lineas adicionadas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Salida: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mostrar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>número de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineas eliminadas</t>
     </r>
   </si>
   <si>
@@ -301,225 +560,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Mostrar el total de LOC del programa No. 2 o versión nueva.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entrada:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> modificar y eliminar lineas de la vesión nueva.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salida:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> numero de lineas modificas y eliminadas, previamente etiquetadas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entradas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Modificar, adicionar y eliminar una linea de código en el segundo programa comprado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salida:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Mostrar en pantalla el efecto realizado, ya sea linea modifica, eliminada o nueva.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entradas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Entrar 2 programas diferentes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salida:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Resultado de lineas comparadas, esta salida depende de los criterios de conteo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entrada:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Subir 1 solo de programa de los 2 a comparar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salida:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Mostrar mensaje de excepción, explicando los sucedido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entrada:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Subir un programa de diferentes nombres o extensiones</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salida:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Mostrar mensaje de error o excepciones</t>
-    </r>
-  </si>
-  <si>
-    <t>CASOS DE PRUEBA CAJA BLANCA</t>
+      <t xml:space="preserve"> línea cn etqueta al inicio de la línea modifica o eliminada.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1125,7 +1167,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1144,7 +1186,7 @@
     </row>
     <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="28" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1238,11 +1280,11 @@
       <c r="F10" s="21"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
       <c r="B11" s="10"/>
       <c r="C11" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
@@ -1253,7 +1295,7 @@
       <c r="A12" s="24"/>
       <c r="B12" s="10"/>
       <c r="C12" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
@@ -1273,7 +1315,7 @@
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
       <c r="C14" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="10"/>
@@ -1284,7 +1326,7 @@
       <c r="A15" s="11"/>
       <c r="B15" s="10"/>
       <c r="C15" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="10"/>
@@ -1297,11 +1339,11 @@
       <c r="E16" s="10"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="10"/>
@@ -1311,7 +1353,7 @@
       <c r="A18" s="11"/>
       <c r="B18" s="10"/>
       <c r="C18" s="15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="10"/>
@@ -1328,7 +1370,7 @@
       <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="10"/>
@@ -1338,7 +1380,7 @@
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="10"/>
@@ -1353,7 +1395,7 @@
         <v>Identificar los LOC adicionadas y eliminadas en el programa</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="10"/>
@@ -1363,7 +1405,7 @@
       <c r="A23" s="11"/>
       <c r="B23" s="10"/>
       <c r="C23" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="10"/>
@@ -1380,7 +1422,7 @@
     <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="C25" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="10"/>
@@ -1388,7 +1430,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="14" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D26" s="21"/>
       <c r="F26" s="21"/>
@@ -1402,7 +1444,7 @@
         <v>Contar los LOC adicionadas y eliminadas en el programa.</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D27" s="21"/>
       <c r="F27" s="21"/>
@@ -1410,7 +1452,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
       <c r="C28" s="12" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D28" s="21"/>
       <c r="F28" s="21"/>
@@ -1424,14 +1466,14 @@
     <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B30" s="10"/>
       <c r="C30" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="21"/>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" s="25" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D31" s="21"/>
       <c r="F31" s="21"/>
@@ -1445,7 +1487,7 @@
         <v>Contar el LOC total en el programa modificado</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D32" s="21"/>
       <c r="F32" s="21"/>
@@ -1453,7 +1495,7 @@
     <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B33" s="10"/>
       <c r="C33" s="27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D33" s="21"/>
       <c r="F33" s="21"/>
@@ -1467,14 +1509,14 @@
         <v>Agregar una etiqueta a la línea, para cada línea modificada o eliminada para indicar el número del cambio</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D34" s="21"/>
       <c r="F34" s="21"/>
     </row>
     <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C35" s="26" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D35" s="21"/>
       <c r="F35" s="21"/>

</xml_diff>

<commit_message>
Correcciones postmortem ciclo 2
</commit_message>
<xml_diff>
--- a/docs/NoteBook/Test plans and data/CASOS DE PRUEBA CICLO2.xlsx
+++ b/docs/NoteBook/Test plans and data/CASOS DE PRUEBA CICLO2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18915" windowHeight="11820"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18915" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="CASOS DE PRUEBA" sheetId="1" r:id="rId1"/>
     <sheet name="REQUERIMIENTOS" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>No</t>
   </si>
@@ -562,13 +562,16 @@
       </rPr>
       <t xml:space="preserve"> línea cn etqueta al inicio de la línea modifica o eliminada.</t>
     </r>
+  </si>
+  <si>
+    <t>TSP Pruebas funcionales.docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,7 +774,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -860,6 +863,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -952,7 +961,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -987,7 +995,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1163,28 +1170,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="7"/>
     <col min="6" max="6" width="31.42578125" style="7" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="26.25">
       <c r="A2" s="28" t="s">
         <v>37</v>
       </c>
@@ -1194,20 +1201,20 @@
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="8"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="13.5" thickBot="1">
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="25.5">
       <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +1235,7 @@
       </c>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" s="19">
         <v>1</v>
       </c>
@@ -1239,14 +1246,18 @@
       <c r="C7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="F7" s="23" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="24"/>
       <c r="B8" s="10"/>
       <c r="C8" s="16"/>
@@ -1255,7 +1266,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="24"/>
       <c r="B9" s="10"/>
       <c r="C9" s="16"/>
@@ -1264,7 +1275,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="60">
       <c r="A10" s="24">
         <v>2</v>
       </c>
@@ -1275,12 +1286,16 @@
       <c r="C10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="D10" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="F10" s="21"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="25.5">
       <c r="A11" s="24"/>
       <c r="B11" s="10"/>
       <c r="C11" s="15" t="s">
@@ -1291,7 +1306,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="25.5">
       <c r="A12" s="24"/>
       <c r="B12" s="10"/>
       <c r="C12" s="15" t="s">
@@ -1302,7 +1317,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="24"/>
       <c r="B13" s="10"/>
       <c r="C13" s="15"/>
@@ -1311,7 +1326,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
       <c r="C14" s="15" t="s">
@@ -1322,7 +1337,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="25.5">
       <c r="A15" s="11"/>
       <c r="B15" s="10"/>
       <c r="C15" s="15" t="s">
@@ -1332,14 +1347,14 @@
       <c r="E15" s="10"/>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="11"/>
       <c r="B16" s="10"/>
       <c r="D16" s="21"/>
       <c r="E16" s="10"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="15" t="s">
@@ -1349,7 +1364,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="25.5">
       <c r="A18" s="11"/>
       <c r="B18" s="10"/>
       <c r="C18" s="15" t="s">
@@ -1359,14 +1374,14 @@
       <c r="E18" s="10"/>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="D19" s="21"/>
       <c r="E19" s="10"/>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="25.5">
       <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="15" t="s">
@@ -1376,7 +1391,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="15" t="s">
@@ -1386,7 +1401,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="60">
       <c r="A22" s="11">
         <v>3</v>
       </c>
@@ -1397,11 +1412,15 @@
       <c r="C22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="F22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="25.5">
       <c r="A23" s="11"/>
       <c r="B23" s="10"/>
       <c r="C23" s="12" t="s">
@@ -1411,7 +1430,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="11"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -1419,7 +1438,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="25.5">
       <c r="A25" s="13"/>
       <c r="C25" s="12" t="s">
         <v>27</v>
@@ -1428,14 +1447,14 @@
       <c r="E25" s="10"/>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="C26" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="21"/>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="60">
       <c r="A27" s="7">
         <v>4</v>
       </c>
@@ -1446,10 +1465,15 @@
       <c r="C27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="B28" s="10"/>
       <c r="C28" s="12" t="s">
         <v>43</v>
@@ -1457,13 +1481,13 @@
       <c r="D28" s="21"/>
       <c r="F28" s="21"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="21"/>
       <c r="F29" s="21"/>
     </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="25.5">
       <c r="B30" s="10"/>
       <c r="C30" s="12" t="s">
         <v>27</v>
@@ -1471,14 +1495,14 @@
       <c r="D30" s="21"/>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="C31" s="25" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="21"/>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="60">
       <c r="A32" s="7">
         <v>5</v>
       </c>
@@ -1489,10 +1513,15 @@
       <c r="C32" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="21"/>
+      <c r="D32" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="25.5">
       <c r="B33" s="10"/>
       <c r="C33" s="27" t="s">
         <v>30</v>
@@ -1500,7 +1529,7 @@
       <c r="D33" s="21"/>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="60">
       <c r="A34" s="7">
         <v>6</v>
       </c>
@@ -1511,10 +1540,15 @@
       <c r="C34" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="21"/>
+      <c r="D34" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="F34" s="21"/>
     </row>
-    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="25.5">
       <c r="C35" s="26" t="s">
         <v>45</v>
       </c>
@@ -1527,21 +1561,33 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" location="REQUERIMIENTOS!A1" display="REQUERIMIENTOS"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E22" r:id="rId3"/>
+    <hyperlink ref="E27" r:id="rId4"/>
+    <hyperlink ref="E32" r:id="rId5"/>
+    <hyperlink ref="E34" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D22" r:id="rId9"/>
+    <hyperlink ref="D27" r:id="rId10"/>
+    <hyperlink ref="D32" r:id="rId11"/>
+    <hyperlink ref="D34" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1549,7 +1595,7 @@
     <col min="4" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1557,7 +1603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1568,7 +1614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1577,7 +1623,7 @@
       </c>
       <c r="C3" s="30"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1586,7 +1632,7 @@
       </c>
       <c r="C4" s="31"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1597,7 +1643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1606,7 +1652,7 @@
       </c>
       <c r="C6" s="33"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1625,12 +1671,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>